<commit_message>
dev environment 2022-09-21 1432
</commit_message>
<xml_diff>
--- a/Tickets/Normal Tickets/Ticket 31445/Testing/Test Plan.xlsx
+++ b/Tickets/Normal Tickets/Ticket 31445/Testing/Test Plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WIP\Tickets\Normal Tickets\Ticket 31445\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Justin's Work\Tickets\Normal Tickets\Ticket 31445\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68671D49-4FCC-4EC9-A8A6-90A8A826890A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C01DBC2-1A5E-45E0-8799-F0E381F4AFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9375" yWindow="-14265" windowWidth="21420" windowHeight="10815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="40" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="97">
   <si>
     <t>Test Case #</t>
   </si>
@@ -337,9 +337,6 @@
   </si>
   <si>
     <t>https://summerclassicsdev.sugarondemand.com/#upsert_CustomQueue/eb8a7530-2f8e-11ed-9557-06be4ff698d4, https://summerclassicsdev.sugarondemand.com/#upsert_CustomQueue/ec92dcd8-2f8e-11ed-ab76-06be4ff698d4, https://summerclassicsdev.sugarondemand.com/#upsert_CustomQueue/ece8af82-2f8e-11ed-853e-06be4ff698d4, https://summerclassicsdev.sugarondemand.com/#upsert_CustomQueue/ed07ab30-2f8e-11ed-aa9c-06be4ff698d4, https://summerclassicsdev.sugarondemand.com/#upsert_CustomQueue/ed2fb184-2f8e-11ed-9a2b-06be4ff698d4, https://summerclassicsdev.sugarondemand.com/#upsert_CustomQueue/ed3e734a-2f8e-11ed-ae13-06be4ff698d4, https://summerclassicsdev.sugarondemand.com/#upsert_CustomQueue/ed43651c-2f8e-11ed-967f-06be4ff698d4, https://summerclassicsdev.sugarondemand.com/#upsert_CustomQueue/ed7c0f70-2f8e-11ed-a5dd-06be4ff698d4, https://summerclassicsdev.sugarondemand.com/#upsert_CustomQueue/ed916f32-2f8e-11ed-9798-06be4ff698d4, https://summerclassicsdev.sugarondemand.com/#upsert_CustomQueue/ed9561be-2f8e-11ed-a843-06be4ff698d4, https://summerclassicsdev.sugarondemand.com/#upsert_CustomQueue/ed9b56a0-2f8e-11ed-b2ab-06be4ff698d4, https://summerclassicsdev.sugarondemand.com/#upsert_CustomQueue/ed9f0106-2f8e-11ed-ab57-06be4ff698d4</t>
-  </si>
-  <si>
-    <t>Justin Pope - 9/9/2022</t>
   </si>
 </sst>
 </file>
@@ -654,32 +651,47 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -687,6 +699,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -705,50 +747,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -757,9 +757,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1102,17 +1099,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="34.7265625" customWidth="1"/>
-    <col min="3" max="3" width="37.7265625" customWidth="1"/>
-    <col min="4" max="4" width="75.54296875" customWidth="1"/>
-    <col min="5" max="5" width="8.81640625" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" customWidth="1"/>
+    <col min="4" max="4" width="75.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="12" customHeight="1">
@@ -1177,129 +1174,120 @@
       </c>
       <c r="E4" s="42"/>
     </row>
-    <row r="5" spans="1:5" ht="13">
-      <c r="A5" s="45"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="53"/>
-    </row>
-    <row r="6" spans="1:5" ht="26">
+    <row r="5" spans="1:5">
+      <c r="A5" s="48"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="50"/>
+    </row>
+    <row r="6" spans="1:5" ht="25.5">
       <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-    </row>
-    <row r="7" spans="1:5" ht="13">
-      <c r="A7" s="45"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="53"/>
-    </row>
-    <row r="8" spans="1:5" ht="13.5">
-      <c r="A8" s="48" t="s">
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="48"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="50"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="48"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="51"/>
-      <c r="E8" s="52"/>
-    </row>
-    <row r="9" spans="1:5" ht="13.5">
-      <c r="A9" s="48" t="s">
+      <c r="D8" s="46"/>
+      <c r="E8" s="47"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="48"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="52"/>
-    </row>
-    <row r="10" spans="1:5" ht="13.5">
-      <c r="A10" s="48" t="s">
+      <c r="D9" s="46"/>
+      <c r="E9" s="47"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-    </row>
-    <row r="11" spans="1:5" ht="13.5">
-      <c r="A11" s="48" t="s">
+      <c r="B10" s="45"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="48"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-    </row>
-    <row r="12" spans="1:5" ht="39">
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+    </row>
+    <row r="12" spans="1:5" ht="38.25">
       <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-    </row>
-    <row r="13" spans="1:5" ht="13">
-      <c r="A13" s="45" t="s">
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="46"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="49"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="9">
         <v>1</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
     </row>
     <row r="15" spans="1:5" ht="32.25" customHeight="1">
       <c r="A15" s="9">
         <v>2</v>
       </c>
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="9">
         <v>3</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D8:E8"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="B15:E15"/>
     <mergeCell ref="B16:E16"/>
@@ -1309,6 +1297,13 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="B12:E12"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1322,78 +1317,78 @@
   </sheetPr>
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="1.453125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="45.1796875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="42.81640625" style="23" customWidth="1"/>
-    <col min="5" max="5" width="96.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.453125" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="3"/>
+    <col min="1" max="1" width="1.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" style="23" customWidth="1"/>
+    <col min="5" max="5" width="96.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.42578125" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="60"/>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="13.5">
-      <c r="A2" s="61" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="75"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1">
+      <c r="A2" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="47">
+      <c r="B2" s="76"/>
+      <c r="C2" s="52">
         <f>'Test Cases'!A2</f>
         <v>1</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-    </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="13.5">
-      <c r="A3" s="61" t="s">
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1">
+      <c r="A3" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="47" t="str">
+      <c r="B3" s="76"/>
+      <c r="C3" s="52" t="str">
         <f>'Test Cases'!B2</f>
         <v>New Quote and Orders</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="47" t="str">
+      <c r="B4" s="76"/>
+      <c r="C4" s="52" t="str">
         <f>'Test Cases'!D2</f>
         <v>1) Access to SQL08 to execute procedures
 2) Access to Syspro
 3) Access to SugarCRM to access the Custom Queue and see the Accounts, Quotes, and Orders</v>
       </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
       <c r="D5" s="20" t="s">
         <v>19</v>
       </c>
@@ -1405,20 +1400,20 @@
       </c>
     </row>
     <row r="6" spans="1:7" s="10" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-    </row>
-    <row r="7" spans="1:7" s="10" customFormat="1" ht="37.5">
-      <c r="A7" s="58">
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+    </row>
+    <row r="7" spans="1:7" s="10" customFormat="1" ht="38.25">
+      <c r="A7" s="73">
         <v>1</v>
       </c>
-      <c r="B7" s="59"/>
+      <c r="B7" s="74"/>
       <c r="C7" s="16" t="s">
         <v>35</v>
       </c>
@@ -1432,11 +1427,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="10" customFormat="1">
-      <c r="A8" s="58">
+    <row r="8" spans="1:7" s="10" customFormat="1" ht="25.5">
+      <c r="A8" s="73">
         <v>2</v>
       </c>
-      <c r="B8" s="59"/>
+      <c r="B8" s="74"/>
       <c r="C8" s="15" t="s">
         <v>39</v>
       </c>
@@ -1449,10 +1444,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" s="10" customFormat="1">
-      <c r="A9" s="58">
+      <c r="A9" s="73">
         <v>3</v>
       </c>
-      <c r="B9" s="59"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="17" t="s">
         <v>44</v>
       </c>
@@ -1464,11 +1459,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="10" customFormat="1" ht="25">
-      <c r="A10" s="58">
+    <row r="10" spans="1:7" s="10" customFormat="1" ht="25.5">
+      <c r="A10" s="73">
         <v>4</v>
       </c>
-      <c r="B10" s="59"/>
+      <c r="B10" s="74"/>
       <c r="C10" s="17" t="s">
         <v>46</v>
       </c>
@@ -1481,10 +1476,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" s="10" customFormat="1">
-      <c r="A11" s="58">
+      <c r="A11" s="73">
         <v>5</v>
       </c>
-      <c r="B11" s="59"/>
+      <c r="B11" s="74"/>
       <c r="C11" s="17" t="s">
         <v>48</v>
       </c>
@@ -1494,21 +1489,21 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="10" customFormat="1" ht="13">
-      <c r="A12" s="57" t="s">
+    <row r="12" spans="1:7" s="10" customFormat="1">
+      <c r="A12" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
     </row>
     <row r="13" spans="1:7" s="10" customFormat="1">
-      <c r="A13" s="70">
+      <c r="A13" s="65">
         <v>1</v>
       </c>
-      <c r="B13" s="71"/>
+      <c r="B13" s="66"/>
       <c r="C13" s="15" t="s">
         <v>49</v>
       </c>
@@ -1517,10 +1512,10 @@
       <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:7" s="10" customFormat="1">
-      <c r="A14" s="70">
+      <c r="A14" s="65">
         <v>2</v>
       </c>
-      <c r="B14" s="71"/>
+      <c r="B14" s="66"/>
       <c r="C14" s="14" t="s">
         <v>50</v>
       </c>
@@ -1533,10 +1528,10 @@
       <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:7" s="10" customFormat="1">
-      <c r="A15" s="72">
+      <c r="A15" s="67">
         <v>3</v>
       </c>
-      <c r="B15" s="73"/>
+      <c r="B15" s="68"/>
       <c r="C15" s="37" t="s">
         <v>51</v>
       </c>
@@ -1545,22 +1540,22 @@
       <c r="F15" s="40"/>
     </row>
     <row r="16" spans="1:7" s="10" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A16" s="74" t="s">
+      <c r="A16" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="75"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="76"/>
-    </row>
-    <row r="17" spans="1:7" s="26" customFormat="1" ht="13">
-      <c r="A17" s="64">
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="58"/>
+    </row>
+    <row r="17" spans="1:7" s="26" customFormat="1">
+      <c r="A17" s="69">
         <f>A7</f>
         <v>1</v>
       </c>
-      <c r="B17" s="65"/>
+      <c r="B17" s="70"/>
       <c r="C17" s="8" t="str">
         <f>C7</f>
         <v>Add ecat orders to system</v>
@@ -1573,8 +1568,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" s="26" customFormat="1" ht="12" customHeight="1">
-      <c r="A18" s="66"/>
-      <c r="B18" s="67"/>
+      <c r="A18" s="63"/>
+      <c r="B18" s="64"/>
       <c r="C18" s="30" t="s">
         <v>52</v>
       </c>
@@ -1584,8 +1579,8 @@
       <c r="G18" s="25"/>
     </row>
     <row r="19" spans="1:7" s="26" customFormat="1" ht="12" customHeight="1">
-      <c r="A19" s="68"/>
-      <c r="B19" s="69"/>
+      <c r="A19" s="61"/>
+      <c r="B19" s="62"/>
       <c r="C19" s="27" t="s">
         <v>66</v>
       </c>
@@ -1595,8 +1590,8 @@
       <c r="G19" s="25"/>
     </row>
     <row r="20" spans="1:7" s="35" customFormat="1" ht="12" customHeight="1">
-      <c r="A20" s="66"/>
-      <c r="B20" s="67"/>
+      <c r="A20" s="63"/>
+      <c r="B20" s="64"/>
       <c r="C20" s="27" t="s">
         <v>63</v>
       </c>
@@ -1606,8 +1601,8 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" s="35" customFormat="1" ht="12" customHeight="1">
-      <c r="A21" s="68"/>
-      <c r="B21" s="69"/>
+      <c r="A21" s="61"/>
+      <c r="B21" s="62"/>
       <c r="C21" s="27" t="s">
         <v>87</v>
       </c>
@@ -1617,8 +1612,8 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" s="35" customFormat="1" ht="12" customHeight="1">
-      <c r="A22" s="68"/>
-      <c r="B22" s="69"/>
+      <c r="A22" s="61"/>
+      <c r="B22" s="62"/>
       <c r="C22" s="27" t="s">
         <v>88</v>
       </c>
@@ -1628,20 +1623,20 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" s="10" customFormat="1">
-      <c r="A23" s="62"/>
-      <c r="B23" s="63"/>
+      <c r="A23" s="54"/>
+      <c r="B23" s="55"/>
       <c r="C23" s="27"/>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
       <c r="F23" s="33"/>
       <c r="G23" s="11"/>
     </row>
-    <row r="24" spans="1:7" s="26" customFormat="1" ht="13">
-      <c r="A24" s="66">
+    <row r="24" spans="1:7" s="26" customFormat="1">
+      <c r="A24" s="63">
         <f>A8</f>
         <v>2</v>
       </c>
-      <c r="B24" s="67"/>
+      <c r="B24" s="64"/>
       <c r="C24" s="30" t="str">
         <f>C8</f>
         <v>Varify that they have been processed</v>
@@ -1652,8 +1647,8 @@
       <c r="G24" s="25"/>
     </row>
     <row r="25" spans="1:7" s="10" customFormat="1">
-      <c r="A25" s="62"/>
-      <c r="B25" s="63"/>
+      <c r="A25" s="54"/>
+      <c r="B25" s="55"/>
       <c r="C25" s="27" t="s">
         <v>64</v>
       </c>
@@ -1665,8 +1660,8 @@
       </c>
     </row>
     <row r="26" spans="1:7" s="10" customFormat="1">
-      <c r="A26" s="62"/>
-      <c r="B26" s="63"/>
+      <c r="A26" s="54"/>
+      <c r="B26" s="55"/>
       <c r="C26" s="27" t="s">
         <v>65</v>
       </c>
@@ -1678,8 +1673,8 @@
       </c>
     </row>
     <row r="27" spans="1:7" s="10" customFormat="1">
-      <c r="A27" s="54"/>
-      <c r="B27" s="55"/>
+      <c r="A27" s="59"/>
+      <c r="B27" s="60"/>
       <c r="C27" s="27" t="s">
         <v>68</v>
       </c>
@@ -1691,8 +1686,8 @@
       </c>
     </row>
     <row r="28" spans="1:7" s="10" customFormat="1">
-      <c r="A28" s="54"/>
-      <c r="B28" s="55"/>
+      <c r="A28" s="59"/>
+      <c r="B28" s="60"/>
       <c r="C28" s="27" t="s">
         <v>67</v>
       </c>
@@ -1706,8 +1701,8 @@
       </c>
     </row>
     <row r="29" spans="1:7" s="10" customFormat="1">
-      <c r="A29" s="54"/>
-      <c r="B29" s="55"/>
+      <c r="A29" s="59"/>
+      <c r="B29" s="60"/>
       <c r="C29" s="27" t="s">
         <v>89</v>
       </c>
@@ -1719,8 +1714,8 @@
       </c>
     </row>
     <row r="30" spans="1:7" s="10" customFormat="1">
-      <c r="A30" s="54"/>
-      <c r="B30" s="55"/>
+      <c r="A30" s="59"/>
+      <c r="B30" s="60"/>
       <c r="C30" s="27" t="s">
         <v>90</v>
       </c>
@@ -1732,8 +1727,8 @@
       </c>
     </row>
     <row r="31" spans="1:7" s="10" customFormat="1">
-      <c r="A31" s="54"/>
-      <c r="B31" s="55"/>
+      <c r="A31" s="59"/>
+      <c r="B31" s="60"/>
       <c r="C31" s="27" t="s">
         <v>91</v>
       </c>
@@ -1747,20 +1742,20 @@
       </c>
     </row>
     <row r="32" spans="1:7" s="10" customFormat="1">
-      <c r="A32" s="62"/>
-      <c r="B32" s="63"/>
+      <c r="A32" s="54"/>
+      <c r="B32" s="55"/>
       <c r="C32" s="27"/>
       <c r="D32" s="27"/>
       <c r="E32" s="27"/>
       <c r="F32" s="33"/>
       <c r="G32" s="11"/>
     </row>
-    <row r="33" spans="1:7" s="26" customFormat="1" ht="13">
-      <c r="A33" s="66">
+    <row r="33" spans="1:7" s="26" customFormat="1">
+      <c r="A33" s="63">
         <f>A9</f>
         <v>3</v>
       </c>
-      <c r="B33" s="67"/>
+      <c r="B33" s="64"/>
       <c r="C33" s="30" t="str">
         <f>C9</f>
         <v>Varify Sugar Integration has picked them up</v>
@@ -1771,8 +1766,8 @@
       <c r="G33" s="25"/>
     </row>
     <row r="34" spans="1:7" s="10" customFormat="1">
-      <c r="A34" s="62"/>
-      <c r="B34" s="63"/>
+      <c r="A34" s="54"/>
+      <c r="B34" s="55"/>
       <c r="C34" s="27" t="s">
         <v>64</v>
       </c>
@@ -1784,8 +1779,8 @@
       </c>
     </row>
     <row r="35" spans="1:7" s="10" customFormat="1">
-      <c r="A35" s="62"/>
-      <c r="B35" s="63"/>
+      <c r="A35" s="54"/>
+      <c r="B35" s="55"/>
       <c r="C35" s="27" t="s">
         <v>65</v>
       </c>
@@ -1797,8 +1792,8 @@
       </c>
     </row>
     <row r="36" spans="1:7" s="10" customFormat="1">
-      <c r="A36" s="54"/>
-      <c r="B36" s="55"/>
+      <c r="A36" s="59"/>
+      <c r="B36" s="60"/>
       <c r="C36" s="27" t="s">
         <v>68</v>
       </c>
@@ -1810,8 +1805,8 @@
       </c>
     </row>
     <row r="37" spans="1:7" s="10" customFormat="1">
-      <c r="A37" s="54"/>
-      <c r="B37" s="55"/>
+      <c r="A37" s="59"/>
+      <c r="B37" s="60"/>
       <c r="C37" s="27" t="s">
         <v>67</v>
       </c>
@@ -1823,8 +1818,8 @@
       </c>
     </row>
     <row r="38" spans="1:7" s="10" customFormat="1">
-      <c r="A38" s="62"/>
-      <c r="B38" s="63"/>
+      <c r="A38" s="54"/>
+      <c r="B38" s="55"/>
       <c r="C38" s="27" t="s">
         <v>89</v>
       </c>
@@ -1837,9 +1832,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="10" customFormat="1" ht="100">
-      <c r="A39" s="62"/>
-      <c r="B39" s="63"/>
+    <row r="39" spans="1:7" s="10" customFormat="1" ht="127.5">
+      <c r="A39" s="54"/>
+      <c r="B39" s="55"/>
       <c r="C39" s="27" t="s">
         <v>90</v>
       </c>
@@ -1852,9 +1847,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="10" customFormat="1" ht="150">
-      <c r="A40" s="62"/>
-      <c r="B40" s="63"/>
+    <row r="40" spans="1:7" s="10" customFormat="1" ht="178.5">
+      <c r="A40" s="54"/>
+      <c r="B40" s="55"/>
       <c r="C40" s="27" t="s">
         <v>91</v>
       </c>
@@ -1868,8 +1863,8 @@
       </c>
     </row>
     <row r="41" spans="1:7" s="10" customFormat="1">
-      <c r="A41" s="62"/>
-      <c r="B41" s="63"/>
+      <c r="A41" s="54"/>
+      <c r="B41" s="55"/>
       <c r="C41" s="27"/>
       <c r="D41" s="27"/>
       <c r="E41" s="27"/>
@@ -1877,8 +1872,8 @@
       <c r="G41" s="11"/>
     </row>
     <row r="42" spans="1:7" s="10" customFormat="1">
-      <c r="A42" s="62"/>
-      <c r="B42" s="63"/>
+      <c r="A42" s="54"/>
+      <c r="B42" s="55"/>
       <c r="C42" s="27"/>
       <c r="D42" s="27"/>
       <c r="E42" s="27"/>
@@ -1886,8 +1881,8 @@
       <c r="G42" s="11"/>
     </row>
     <row r="43" spans="1:7" s="10" customFormat="1">
-      <c r="A43" s="62"/>
-      <c r="B43" s="63"/>
+      <c r="A43" s="54"/>
+      <c r="B43" s="55"/>
       <c r="C43" s="27"/>
       <c r="D43" s="27"/>
       <c r="E43" s="27"/>
@@ -1895,8 +1890,8 @@
       <c r="G43" s="11"/>
     </row>
     <row r="44" spans="1:7" s="10" customFormat="1">
-      <c r="A44" s="62"/>
-      <c r="B44" s="63"/>
+      <c r="A44" s="54"/>
+      <c r="B44" s="55"/>
       <c r="C44" s="27"/>
       <c r="D44" s="27"/>
       <c r="E44" s="27"/>
@@ -1904,8 +1899,8 @@
       <c r="G44" s="11"/>
     </row>
     <row r="45" spans="1:7" s="10" customFormat="1">
-      <c r="A45" s="62"/>
-      <c r="B45" s="63"/>
+      <c r="A45" s="54"/>
+      <c r="B45" s="55"/>
       <c r="C45" s="27"/>
       <c r="D45" s="27"/>
       <c r="E45" s="27"/>
@@ -1913,8 +1908,8 @@
       <c r="G45" s="11"/>
     </row>
     <row r="46" spans="1:7" s="10" customFormat="1">
-      <c r="A46" s="62"/>
-      <c r="B46" s="63"/>
+      <c r="A46" s="54"/>
+      <c r="B46" s="55"/>
       <c r="C46" s="27"/>
       <c r="D46" s="27"/>
       <c r="E46" s="27"/>
@@ -1922,8 +1917,8 @@
       <c r="G46" s="11"/>
     </row>
     <row r="47" spans="1:7" s="10" customFormat="1">
-      <c r="A47" s="62"/>
-      <c r="B47" s="63"/>
+      <c r="A47" s="54"/>
+      <c r="B47" s="55"/>
       <c r="C47" s="27"/>
       <c r="D47" s="27"/>
       <c r="E47" s="27"/>
@@ -1931,8 +1926,8 @@
       <c r="G47" s="11"/>
     </row>
     <row r="48" spans="1:7" s="10" customFormat="1">
-      <c r="A48" s="62"/>
-      <c r="B48" s="63"/>
+      <c r="A48" s="54"/>
+      <c r="B48" s="55"/>
       <c r="C48" s="27"/>
       <c r="D48" s="27"/>
       <c r="E48" s="27"/>
@@ -1940,8 +1935,8 @@
       <c r="G48" s="11"/>
     </row>
     <row r="49" spans="1:7" s="10" customFormat="1">
-      <c r="A49" s="62"/>
-      <c r="B49" s="63"/>
+      <c r="A49" s="54"/>
+      <c r="B49" s="55"/>
       <c r="C49" s="27"/>
       <c r="D49" s="27"/>
       <c r="E49" s="27"/>
@@ -1949,8 +1944,8 @@
       <c r="G49" s="11"/>
     </row>
     <row r="50" spans="1:7" s="10" customFormat="1">
-      <c r="A50" s="62"/>
-      <c r="B50" s="63"/>
+      <c r="A50" s="54"/>
+      <c r="B50" s="55"/>
       <c r="C50" s="27"/>
       <c r="D50" s="27"/>
       <c r="E50" s="27"/>
@@ -1958,8 +1953,8 @@
       <c r="G50" s="11"/>
     </row>
     <row r="51" spans="1:7" s="10" customFormat="1">
-      <c r="A51" s="62"/>
-      <c r="B51" s="63"/>
+      <c r="A51" s="54"/>
+      <c r="B51" s="55"/>
       <c r="C51" s="27"/>
       <c r="D51" s="27"/>
       <c r="E51" s="27"/>
@@ -1967,8 +1962,8 @@
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" s="10" customFormat="1">
-      <c r="A52" s="62"/>
-      <c r="B52" s="63"/>
+      <c r="A52" s="54"/>
+      <c r="B52" s="55"/>
       <c r="C52" s="27"/>
       <c r="D52" s="27"/>
       <c r="E52" s="27"/>
@@ -1976,8 +1971,8 @@
       <c r="G52" s="11"/>
     </row>
     <row r="53" spans="1:7" s="10" customFormat="1">
-      <c r="A53" s="62"/>
-      <c r="B53" s="63"/>
+      <c r="A53" s="54"/>
+      <c r="B53" s="55"/>
       <c r="C53" s="27"/>
       <c r="D53" s="27"/>
       <c r="E53" s="27"/>
@@ -1985,8 +1980,8 @@
       <c r="G53" s="11"/>
     </row>
     <row r="54" spans="1:7" s="10" customFormat="1">
-      <c r="A54" s="62"/>
-      <c r="B54" s="63"/>
+      <c r="A54" s="54"/>
+      <c r="B54" s="55"/>
       <c r="C54" s="27"/>
       <c r="D54" s="27"/>
       <c r="E54" s="27"/>
@@ -1994,8 +1989,8 @@
       <c r="G54" s="11"/>
     </row>
     <row r="55" spans="1:7" s="10" customFormat="1">
-      <c r="A55" s="62"/>
-      <c r="B55" s="63"/>
+      <c r="A55" s="54"/>
+      <c r="B55" s="55"/>
       <c r="C55" s="27"/>
       <c r="D55" s="27"/>
       <c r="E55" s="27"/>
@@ -2003,8 +1998,8 @@
       <c r="G55" s="11"/>
     </row>
     <row r="56" spans="1:7" s="10" customFormat="1">
-      <c r="A56" s="62"/>
-      <c r="B56" s="63"/>
+      <c r="A56" s="54"/>
+      <c r="B56" s="55"/>
       <c r="C56" s="27"/>
       <c r="D56" s="27"/>
       <c r="E56" s="27"/>
@@ -2012,8 +2007,8 @@
       <c r="G56" s="11"/>
     </row>
     <row r="57" spans="1:7" s="10" customFormat="1">
-      <c r="A57" s="62"/>
-      <c r="B57" s="63"/>
+      <c r="A57" s="54"/>
+      <c r="B57" s="55"/>
       <c r="C57" s="27"/>
       <c r="D57" s="28"/>
       <c r="E57" s="29"/>
@@ -2021,8 +2016,8 @@
       <c r="G57" s="11"/>
     </row>
     <row r="58" spans="1:7" s="10" customFormat="1">
-      <c r="A58" s="62"/>
-      <c r="B58" s="63"/>
+      <c r="A58" s="54"/>
+      <c r="B58" s="55"/>
       <c r="C58" s="27"/>
       <c r="D58" s="28"/>
       <c r="E58" s="29"/>
@@ -2030,8 +2025,8 @@
       <c r="G58" s="11"/>
     </row>
     <row r="59" spans="1:7" s="10" customFormat="1">
-      <c r="A59" s="62"/>
-      <c r="B59" s="63"/>
+      <c r="A59" s="54"/>
+      <c r="B59" s="55"/>
       <c r="C59" s="27"/>
       <c r="D59" s="28"/>
       <c r="E59" s="29"/>
@@ -2039,8 +2034,8 @@
       <c r="G59" s="11"/>
     </row>
     <row r="60" spans="1:7" s="10" customFormat="1">
-      <c r="A60" s="62"/>
-      <c r="B60" s="63"/>
+      <c r="A60" s="54"/>
+      <c r="B60" s="55"/>
       <c r="C60" s="27"/>
       <c r="D60" s="28"/>
       <c r="E60" s="29"/>
@@ -2048,8 +2043,8 @@
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" s="10" customFormat="1">
-      <c r="A61" s="62"/>
-      <c r="B61" s="63"/>
+      <c r="A61" s="54"/>
+      <c r="B61" s="55"/>
       <c r="C61" s="27"/>
       <c r="D61" s="28"/>
       <c r="E61" s="29"/>
@@ -2057,8 +2052,8 @@
       <c r="G61" s="11"/>
     </row>
     <row r="62" spans="1:7" s="10" customFormat="1">
-      <c r="A62" s="62"/>
-      <c r="B62" s="63"/>
+      <c r="A62" s="54"/>
+      <c r="B62" s="55"/>
       <c r="C62" s="27"/>
       <c r="D62" s="28"/>
       <c r="E62" s="29"/>
@@ -2067,6 +2062,55 @@
     </row>
   </sheetData>
   <mergeCells count="65">
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
     <mergeCell ref="A62:B62"/>
     <mergeCell ref="A16:G16"/>
     <mergeCell ref="A28:B28"/>
@@ -2083,55 +2127,6 @@
     <mergeCell ref="A55:B55"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A26:B26"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2148,73 +2143,73 @@
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="1.453125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="45.1796875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="42.81640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="42.81640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="42.453125" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="3"/>
+    <col min="1" max="1" width="1.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="42.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="42.42578125" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="60"/>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="13.5">
-      <c r="A2" s="61" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="75"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1">
+      <c r="A2" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="47">
+      <c r="B2" s="76"/>
+      <c r="C2" s="52">
         <f>'Test Cases'!A3</f>
         <v>2</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-    </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="13.5">
-      <c r="A3" s="61" t="s">
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1">
+      <c r="A3" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="47" t="str">
+      <c r="B3" s="76"/>
+      <c r="C3" s="52" t="str">
         <f>'Test Cases'!B3</f>
         <v>Updated Quote and Orders</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="47" t="str">
+      <c r="B4" s="76"/>
+      <c r="C4" s="52" t="str">
         <f>'Test Cases'!D3</f>
         <v>1) Access to SQL08 to execute procedures
 2) Access to SQL08 server to see Talend logs
 3) Access to SugarCRM to access the Custom Queue and see the Accounts, Quotes, and Orders</v>
       </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
       <c r="D5" s="19" t="s">
         <v>19</v>
       </c>
@@ -2226,20 +2221,20 @@
       </c>
     </row>
     <row r="6" spans="1:7" s="10" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-    </row>
-    <row r="7" spans="1:7" s="10" customFormat="1" ht="25">
-      <c r="A7" s="58">
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+    </row>
+    <row r="7" spans="1:7" s="10" customFormat="1" ht="25.5">
+      <c r="A7" s="73">
         <v>1</v>
       </c>
-      <c r="B7" s="59"/>
+      <c r="B7" s="74"/>
       <c r="C7" s="17" t="s">
         <v>54</v>
       </c>
@@ -2251,11 +2246,11 @@
       </c>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:7" s="10" customFormat="1" ht="25">
-      <c r="A8" s="58">
+    <row r="8" spans="1:7" s="10" customFormat="1" ht="25.5">
+      <c r="A8" s="73">
         <v>2</v>
       </c>
-      <c r="B8" s="59"/>
+      <c r="B8" s="74"/>
       <c r="C8" s="17" t="s">
         <v>57</v>
       </c>
@@ -2269,21 +2264,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="10" customFormat="1" ht="13">
-      <c r="A9" s="57" t="s">
+    <row r="9" spans="1:7" s="10" customFormat="1">
+      <c r="A9" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
     </row>
     <row r="10" spans="1:7" s="10" customFormat="1">
-      <c r="A10" s="70">
+      <c r="A10" s="65">
         <v>1</v>
       </c>
-      <c r="B10" s="71"/>
+      <c r="B10" s="66"/>
       <c r="C10" s="17" t="s">
         <v>49</v>
       </c>
@@ -2292,10 +2287,10 @@
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:7" s="10" customFormat="1">
-      <c r="A11" s="70">
+      <c r="A11" s="65">
         <v>2</v>
       </c>
-      <c r="B11" s="71"/>
+      <c r="B11" s="66"/>
       <c r="C11" s="14" t="s">
         <v>50</v>
       </c>
@@ -2308,10 +2303,10 @@
       <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:7" s="10" customFormat="1">
-      <c r="A12" s="72">
+      <c r="A12" s="67">
         <v>3</v>
       </c>
-      <c r="B12" s="73"/>
+      <c r="B12" s="68"/>
       <c r="C12" s="37" t="s">
         <v>51</v>
       </c>
@@ -2320,22 +2315,22 @@
       <c r="F12" s="40"/>
     </row>
     <row r="13" spans="1:7" s="10" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="75"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="76"/>
-    </row>
-    <row r="14" spans="1:7" s="26" customFormat="1" ht="13">
-      <c r="A14" s="64" t="str">
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="58"/>
+    </row>
+    <row r="14" spans="1:7" s="26" customFormat="1">
+      <c r="A14" s="69" t="str">
         <f>A4</f>
         <v>Test  Consideration</v>
       </c>
-      <c r="B14" s="65"/>
+      <c r="B14" s="70"/>
       <c r="C14" s="8" t="str">
         <f>C7</f>
         <v>Change data</v>
@@ -2346,8 +2341,8 @@
       <c r="G14" s="25"/>
     </row>
     <row r="15" spans="1:7" s="26" customFormat="1" ht="12" customHeight="1">
-      <c r="A15" s="66"/>
-      <c r="B15" s="67"/>
+      <c r="A15" s="63"/>
+      <c r="B15" s="64"/>
       <c r="C15" s="27" t="s">
         <v>59</v>
       </c>
@@ -2359,8 +2354,8 @@
       <c r="G15" s="25"/>
     </row>
     <row r="16" spans="1:7" s="35" customFormat="1" ht="12" customHeight="1">
-      <c r="A16" s="66"/>
-      <c r="B16" s="67"/>
+      <c r="A16" s="63"/>
+      <c r="B16" s="64"/>
       <c r="C16" s="27" t="s">
         <v>60</v>
       </c>
@@ -2372,20 +2367,20 @@
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" s="10" customFormat="1">
-      <c r="A17" s="62"/>
-      <c r="B17" s="63"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="55"/>
       <c r="C17" s="27"/>
       <c r="D17" s="27"/>
       <c r="E17" s="27"/>
       <c r="F17" s="33"/>
       <c r="G17" s="11"/>
     </row>
-    <row r="18" spans="1:7" s="26" customFormat="1" ht="13">
-      <c r="A18" s="66" t="str">
+    <row r="18" spans="1:7" s="26" customFormat="1">
+      <c r="A18" s="63" t="str">
         <f>A5</f>
         <v>Test Condition</v>
       </c>
-      <c r="B18" s="67"/>
+      <c r="B18" s="64"/>
       <c r="C18" s="8" t="str">
         <f>C8</f>
         <v>Verify in Sugar CRM</v>
@@ -2398,8 +2393,8 @@
       </c>
     </row>
     <row r="19" spans="1:7" s="10" customFormat="1">
-      <c r="A19" s="62"/>
-      <c r="B19" s="63"/>
+      <c r="A19" s="54"/>
+      <c r="B19" s="55"/>
       <c r="C19" s="27" t="s">
         <v>59</v>
       </c>
@@ -2411,8 +2406,8 @@
       </c>
     </row>
     <row r="20" spans="1:7" s="10" customFormat="1">
-      <c r="A20" s="62"/>
-      <c r="B20" s="63"/>
+      <c r="A20" s="54"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="27" t="s">
         <v>60</v>
       </c>
@@ -2424,17 +2419,17 @@
       </c>
     </row>
     <row r="21" spans="1:7" s="10" customFormat="1">
-      <c r="A21" s="62"/>
-      <c r="B21" s="63"/>
+      <c r="A21" s="54"/>
+      <c r="B21" s="55"/>
       <c r="C21" s="27"/>
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
       <c r="F21" s="33"/>
       <c r="G21" s="11"/>
     </row>
-    <row r="22" spans="1:7" s="26" customFormat="1" ht="13">
-      <c r="A22" s="66"/>
-      <c r="B22" s="67"/>
+    <row r="22" spans="1:7" s="26" customFormat="1">
+      <c r="A22" s="63"/>
+      <c r="B22" s="64"/>
       <c r="C22" s="30"/>
       <c r="D22" s="30"/>
       <c r="E22" s="30"/>
@@ -2442,8 +2437,8 @@
       <c r="G22" s="25"/>
     </row>
     <row r="23" spans="1:7" s="10" customFormat="1">
-      <c r="A23" s="62"/>
-      <c r="B23" s="63"/>
+      <c r="A23" s="54"/>
+      <c r="B23" s="55"/>
       <c r="C23" s="27"/>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
@@ -2451,8 +2446,8 @@
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" s="10" customFormat="1">
-      <c r="A24" s="62"/>
-      <c r="B24" s="63"/>
+      <c r="A24" s="54"/>
+      <c r="B24" s="55"/>
       <c r="C24" s="27"/>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
@@ -2460,8 +2455,8 @@
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" s="10" customFormat="1">
-      <c r="A25" s="62"/>
-      <c r="B25" s="63"/>
+      <c r="A25" s="54"/>
+      <c r="B25" s="55"/>
       <c r="C25" s="27"/>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
@@ -2469,8 +2464,8 @@
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" s="10" customFormat="1">
-      <c r="A26" s="62"/>
-      <c r="B26" s="63"/>
+      <c r="A26" s="54"/>
+      <c r="B26" s="55"/>
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
       <c r="E26" s="27"/>
@@ -2478,8 +2473,8 @@
       <c r="G26" s="11"/>
     </row>
     <row r="27" spans="1:7" s="10" customFormat="1">
-      <c r="A27" s="62"/>
-      <c r="B27" s="63"/>
+      <c r="A27" s="54"/>
+      <c r="B27" s="55"/>
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
       <c r="E27" s="27"/>
@@ -2487,8 +2482,8 @@
       <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:7" s="10" customFormat="1">
-      <c r="A28" s="62"/>
-      <c r="B28" s="63"/>
+      <c r="A28" s="54"/>
+      <c r="B28" s="55"/>
       <c r="C28" s="27"/>
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
@@ -2496,8 +2491,8 @@
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" s="10" customFormat="1">
-      <c r="A29" s="62"/>
-      <c r="B29" s="63"/>
+      <c r="A29" s="54"/>
+      <c r="B29" s="55"/>
       <c r="C29" s="27"/>
       <c r="D29" s="27"/>
       <c r="E29" s="27"/>
@@ -2505,8 +2500,8 @@
       <c r="G29" s="11"/>
     </row>
     <row r="30" spans="1:7" s="10" customFormat="1">
-      <c r="A30" s="62"/>
-      <c r="B30" s="63"/>
+      <c r="A30" s="54"/>
+      <c r="B30" s="55"/>
       <c r="C30" s="27"/>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
@@ -2514,8 +2509,8 @@
       <c r="G30" s="11"/>
     </row>
     <row r="31" spans="1:7" s="10" customFormat="1">
-      <c r="A31" s="62"/>
-      <c r="B31" s="63"/>
+      <c r="A31" s="54"/>
+      <c r="B31" s="55"/>
       <c r="C31" s="27"/>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
@@ -2523,8 +2518,8 @@
       <c r="G31" s="11"/>
     </row>
     <row r="32" spans="1:7" s="10" customFormat="1">
-      <c r="A32" s="62"/>
-      <c r="B32" s="63"/>
+      <c r="A32" s="54"/>
+      <c r="B32" s="55"/>
       <c r="C32" s="27"/>
       <c r="D32" s="27"/>
       <c r="E32" s="27"/>
@@ -2532,8 +2527,8 @@
       <c r="G32" s="11"/>
     </row>
     <row r="33" spans="1:7" s="10" customFormat="1">
-      <c r="A33" s="62"/>
-      <c r="B33" s="63"/>
+      <c r="A33" s="54"/>
+      <c r="B33" s="55"/>
       <c r="C33" s="27"/>
       <c r="D33" s="27"/>
       <c r="E33" s="27"/>
@@ -2541,8 +2536,8 @@
       <c r="G33" s="11"/>
     </row>
     <row r="34" spans="1:7" s="10" customFormat="1">
-      <c r="A34" s="62"/>
-      <c r="B34" s="63"/>
+      <c r="A34" s="54"/>
+      <c r="B34" s="55"/>
       <c r="C34" s="27"/>
       <c r="D34" s="27"/>
       <c r="E34" s="27"/>
@@ -2550,8 +2545,8 @@
       <c r="G34" s="11"/>
     </row>
     <row r="35" spans="1:7" s="10" customFormat="1">
-      <c r="A35" s="62"/>
-      <c r="B35" s="63"/>
+      <c r="A35" s="54"/>
+      <c r="B35" s="55"/>
       <c r="C35" s="27"/>
       <c r="D35" s="27"/>
       <c r="E35" s="27"/>
@@ -2559,8 +2554,8 @@
       <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" s="10" customFormat="1">
-      <c r="A36" s="62"/>
-      <c r="B36" s="63"/>
+      <c r="A36" s="54"/>
+      <c r="B36" s="55"/>
       <c r="C36" s="27"/>
       <c r="D36" s="27"/>
       <c r="E36" s="27"/>
@@ -2568,8 +2563,8 @@
       <c r="G36" s="11"/>
     </row>
     <row r="37" spans="1:7" s="10" customFormat="1">
-      <c r="A37" s="62"/>
-      <c r="B37" s="63"/>
+      <c r="A37" s="54"/>
+      <c r="B37" s="55"/>
       <c r="C37" s="27"/>
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
@@ -2577,8 +2572,8 @@
       <c r="G37" s="11"/>
     </row>
     <row r="38" spans="1:7" s="10" customFormat="1">
-      <c r="A38" s="62"/>
-      <c r="B38" s="63"/>
+      <c r="A38" s="54"/>
+      <c r="B38" s="55"/>
       <c r="C38" s="27"/>
       <c r="D38" s="27"/>
       <c r="E38" s="27"/>
@@ -2586,8 +2581,8 @@
       <c r="G38" s="11"/>
     </row>
     <row r="39" spans="1:7" s="10" customFormat="1">
-      <c r="A39" s="62"/>
-      <c r="B39" s="63"/>
+      <c r="A39" s="54"/>
+      <c r="B39" s="55"/>
       <c r="C39" s="27"/>
       <c r="D39" s="27"/>
       <c r="E39" s="27"/>
@@ -2595,8 +2590,8 @@
       <c r="G39" s="11"/>
     </row>
     <row r="40" spans="1:7" s="10" customFormat="1">
-      <c r="A40" s="62"/>
-      <c r="B40" s="63"/>
+      <c r="A40" s="54"/>
+      <c r="B40" s="55"/>
       <c r="C40" s="27"/>
       <c r="D40" s="27"/>
       <c r="E40" s="27"/>
@@ -2604,8 +2599,8 @@
       <c r="G40" s="11"/>
     </row>
     <row r="41" spans="1:7" s="10" customFormat="1">
-      <c r="A41" s="62"/>
-      <c r="B41" s="63"/>
+      <c r="A41" s="54"/>
+      <c r="B41" s="55"/>
       <c r="C41" s="27"/>
       <c r="D41" s="27"/>
       <c r="E41" s="27"/>
@@ -2613,8 +2608,8 @@
       <c r="G41" s="11"/>
     </row>
     <row r="42" spans="1:7" s="10" customFormat="1">
-      <c r="A42" s="62"/>
-      <c r="B42" s="63"/>
+      <c r="A42" s="54"/>
+      <c r="B42" s="55"/>
       <c r="C42" s="27"/>
       <c r="D42" s="27"/>
       <c r="E42" s="27"/>
@@ -2622,8 +2617,8 @@
       <c r="G42" s="11"/>
     </row>
     <row r="43" spans="1:7" s="10" customFormat="1">
-      <c r="A43" s="62"/>
-      <c r="B43" s="63"/>
+      <c r="A43" s="54"/>
+      <c r="B43" s="55"/>
       <c r="C43" s="27"/>
       <c r="D43" s="27"/>
       <c r="E43" s="27"/>
@@ -2631,8 +2626,8 @@
       <c r="G43" s="11"/>
     </row>
     <row r="44" spans="1:7" s="10" customFormat="1">
-      <c r="A44" s="62"/>
-      <c r="B44" s="63"/>
+      <c r="A44" s="54"/>
+      <c r="B44" s="55"/>
       <c r="C44" s="27"/>
       <c r="D44" s="27"/>
       <c r="E44" s="27"/>
@@ -2640,8 +2635,8 @@
       <c r="G44" s="11"/>
     </row>
     <row r="45" spans="1:7" s="10" customFormat="1">
-      <c r="A45" s="62"/>
-      <c r="B45" s="63"/>
+      <c r="A45" s="54"/>
+      <c r="B45" s="55"/>
       <c r="C45" s="27"/>
       <c r="D45" s="27"/>
       <c r="E45" s="27"/>
@@ -2649,8 +2644,8 @@
       <c r="G45" s="11"/>
     </row>
     <row r="46" spans="1:7" s="10" customFormat="1">
-      <c r="A46" s="62"/>
-      <c r="B46" s="63"/>
+      <c r="A46" s="54"/>
+      <c r="B46" s="55"/>
       <c r="C46" s="27"/>
       <c r="D46" s="28"/>
       <c r="E46" s="29"/>
@@ -2658,8 +2653,8 @@
       <c r="G46" s="11"/>
     </row>
     <row r="47" spans="1:7" s="10" customFormat="1">
-      <c r="A47" s="62"/>
-      <c r="B47" s="63"/>
+      <c r="A47" s="54"/>
+      <c r="B47" s="55"/>
       <c r="C47" s="27"/>
       <c r="D47" s="28"/>
       <c r="E47" s="29"/>
@@ -2667,8 +2662,8 @@
       <c r="G47" s="11"/>
     </row>
     <row r="48" spans="1:7" s="10" customFormat="1">
-      <c r="A48" s="62"/>
-      <c r="B48" s="63"/>
+      <c r="A48" s="54"/>
+      <c r="B48" s="55"/>
       <c r="C48" s="27"/>
       <c r="D48" s="28"/>
       <c r="E48" s="29"/>
@@ -2676,8 +2671,8 @@
       <c r="G48" s="11"/>
     </row>
     <row r="49" spans="1:7" s="10" customFormat="1">
-      <c r="A49" s="62"/>
-      <c r="B49" s="63"/>
+      <c r="A49" s="54"/>
+      <c r="B49" s="55"/>
       <c r="C49" s="27"/>
       <c r="D49" s="28"/>
       <c r="E49" s="29"/>
@@ -2685,8 +2680,8 @@
       <c r="G49" s="11"/>
     </row>
     <row r="50" spans="1:7" s="10" customFormat="1">
-      <c r="A50" s="62"/>
-      <c r="B50" s="63"/>
+      <c r="A50" s="54"/>
+      <c r="B50" s="55"/>
       <c r="C50" s="27"/>
       <c r="D50" s="28"/>
       <c r="E50" s="29"/>
@@ -2694,8 +2689,8 @@
       <c r="G50" s="11"/>
     </row>
     <row r="51" spans="1:7" s="10" customFormat="1">
-      <c r="A51" s="62"/>
-      <c r="B51" s="63"/>
+      <c r="A51" s="54"/>
+      <c r="B51" s="55"/>
       <c r="C51" s="27"/>
       <c r="D51" s="28"/>
       <c r="E51" s="29"/>
@@ -2716,30 +2711,23 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A19:B19"/>
@@ -2753,23 +2741,30 @@
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2784,72 +2779,72 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="1.453125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="45.1796875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="42.81640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="42.81640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="42.453125" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="3"/>
+    <col min="1" max="1" width="1.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="42.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="42.42578125" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="60"/>
-    </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="13.5">
-      <c r="A2" s="61" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="75"/>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1">
+      <c r="A2" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="47">
+      <c r="B2" s="76"/>
+      <c r="C2" s="52">
         <f>'Test Cases'!A4</f>
         <v>3</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="13.5">
-      <c r="A3" s="61" t="s">
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1">
+      <c r="A3" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="47" t="str">
+      <c r="B3" s="76"/>
+      <c r="C3" s="52" t="str">
         <f>'Test Cases'!B4</f>
         <v>Compare .json data to CSV data</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="57.75" customHeight="1">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="47" t="str">
+      <c r="B4" s="76"/>
+      <c r="C4" s="52" t="str">
         <f>'Test Cases'!D4</f>
         <v>1) Access to SQL08 to execute procedures
 2) Access to see the files generated by the two processes</v>
       </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
       <c r="D5" s="44" t="s">
         <v>19</v>
       </c>
@@ -2861,20 +2856,20 @@
       </c>
     </row>
     <row r="6" spans="1:6" s="10" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
     </row>
     <row r="7" spans="1:6" s="10" customFormat="1">
-      <c r="A7" s="58">
+      <c r="A7" s="73">
         <v>1</v>
       </c>
-      <c r="B7" s="59"/>
+      <c r="B7" s="74"/>
       <c r="C7" s="42" t="s">
         <v>72</v>
       </c>
@@ -2889,10 +2884,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" s="10" customFormat="1">
-      <c r="A8" s="58">
+      <c r="A8" s="73">
         <v>2</v>
       </c>
-      <c r="B8" s="59"/>
+      <c r="B8" s="74"/>
       <c r="C8" s="42" t="s">
         <v>76</v>
       </c>
@@ -2905,10 +2900,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" s="10" customFormat="1">
-      <c r="A9" s="58">
+      <c r="A9" s="73">
         <v>3</v>
       </c>
-      <c r="B9" s="59"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="42" t="s">
         <v>79</v>
       </c>
@@ -2916,11 +2911,11 @@
       <c r="E9" s="7"/>
       <c r="F9" s="43"/>
     </row>
-    <row r="10" spans="1:6" s="10" customFormat="1" ht="25">
-      <c r="A10" s="58">
+    <row r="10" spans="1:6" s="10" customFormat="1" ht="25.5">
+      <c r="A10" s="73">
         <v>4</v>
       </c>
-      <c r="B10" s="59"/>
+      <c r="B10" s="74"/>
       <c r="C10" s="42" t="s">
         <v>80</v>
       </c>
@@ -2932,21 +2927,21 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="10" customFormat="1" ht="13">
-      <c r="A11" s="57" t="s">
+    <row r="11" spans="1:6" s="10" customFormat="1">
+      <c r="A11" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="72"/>
     </row>
     <row r="12" spans="1:6" s="10" customFormat="1">
-      <c r="A12" s="70">
+      <c r="A12" s="65">
         <v>1</v>
       </c>
-      <c r="B12" s="71"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="42" t="s">
         <v>49</v>
       </c>
@@ -2955,10 +2950,10 @@
       <c r="F12" s="43"/>
     </row>
     <row r="13" spans="1:6" s="10" customFormat="1">
-      <c r="A13" s="70">
+      <c r="A13" s="65">
         <v>2</v>
       </c>
-      <c r="B13" s="71"/>
+      <c r="B13" s="66"/>
       <c r="C13" s="14" t="s">
         <v>50</v>
       </c>
@@ -2971,10 +2966,10 @@
       <c r="F13" s="43"/>
     </row>
     <row r="14" spans="1:6" s="10" customFormat="1">
-      <c r="A14" s="72">
+      <c r="A14" s="67">
         <v>3</v>
       </c>
-      <c r="B14" s="73"/>
+      <c r="B14" s="68"/>
       <c r="C14" s="37" t="s">
         <v>51</v>
       </c>
@@ -2983,18 +2978,18 @@
       <c r="F14" s="40"/>
     </row>
     <row r="15" spans="1:6" s="10" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A15" s="78" t="s">
+      <c r="A15" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="78"/>
-      <c r="C15" s="78"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-    </row>
-    <row r="16" spans="1:6" s="26" customFormat="1" ht="25">
-      <c r="A16" s="79"/>
-      <c r="B16" s="79"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="79"/>
+      <c r="F15" s="79"/>
+    </row>
+    <row r="16" spans="1:6" s="26" customFormat="1" ht="25.5">
+      <c r="A16" s="80"/>
+      <c r="B16" s="80"/>
       <c r="C16" s="42" t="s">
         <v>83</v>
       </c>
@@ -3002,9 +2997,9 @@
       <c r="E16" s="25"/>
       <c r="F16" s="25"/>
     </row>
-    <row r="17" spans="1:6" s="26" customFormat="1" ht="25">
-      <c r="A17" s="77"/>
-      <c r="B17" s="77"/>
+    <row r="17" spans="1:6" s="26" customFormat="1" ht="25.5">
+      <c r="A17" s="78"/>
+      <c r="B17" s="78"/>
       <c r="C17" s="27" t="s">
         <v>84</v>
       </c>
@@ -3017,288 +3012,288 @@
       <c r="F17" s="30"/>
     </row>
     <row r="18" spans="1:6" s="35" customFormat="1" ht="12" customHeight="1">
-      <c r="A18" s="77"/>
-      <c r="B18" s="77"/>
+      <c r="A18" s="78"/>
+      <c r="B18" s="78"/>
       <c r="C18" s="27"/>
       <c r="D18" s="36"/>
       <c r="E18" s="27"/>
       <c r="F18" s="27"/>
     </row>
     <row r="19" spans="1:6" s="10" customFormat="1">
-      <c r="A19" s="80"/>
-      <c r="B19" s="80"/>
+      <c r="A19" s="77"/>
+      <c r="B19" s="77"/>
       <c r="C19" s="27"/>
       <c r="D19" s="27"/>
       <c r="E19" s="27"/>
       <c r="F19" s="27"/>
     </row>
-    <row r="20" spans="1:6" s="26" customFormat="1" ht="13">
-      <c r="A20" s="77"/>
-      <c r="B20" s="77"/>
+    <row r="20" spans="1:6" s="26" customFormat="1">
+      <c r="A20" s="78"/>
+      <c r="B20" s="78"/>
       <c r="C20" s="8"/>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
       <c r="F20" s="30"/>
     </row>
     <row r="21" spans="1:6" s="10" customFormat="1">
-      <c r="A21" s="80"/>
-      <c r="B21" s="80"/>
+      <c r="A21" s="77"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="27"/>
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
       <c r="F21" s="27"/>
     </row>
     <row r="22" spans="1:6" s="10" customFormat="1">
-      <c r="A22" s="80"/>
-      <c r="B22" s="80"/>
+      <c r="A22" s="77"/>
+      <c r="B22" s="77"/>
       <c r="C22" s="27"/>
       <c r="D22" s="27"/>
       <c r="E22" s="27"/>
       <c r="F22" s="27"/>
     </row>
     <row r="23" spans="1:6" s="10" customFormat="1">
-      <c r="A23" s="80"/>
-      <c r="B23" s="80"/>
+      <c r="A23" s="77"/>
+      <c r="B23" s="77"/>
       <c r="C23" s="27"/>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
       <c r="F23" s="27"/>
     </row>
-    <row r="24" spans="1:6" s="26" customFormat="1" ht="13">
-      <c r="A24" s="77"/>
-      <c r="B24" s="77"/>
+    <row r="24" spans="1:6" s="26" customFormat="1">
+      <c r="A24" s="78"/>
+      <c r="B24" s="78"/>
       <c r="C24" s="30"/>
       <c r="D24" s="30"/>
       <c r="E24" s="30"/>
       <c r="F24" s="30"/>
     </row>
     <row r="25" spans="1:6" s="10" customFormat="1">
-      <c r="A25" s="80"/>
-      <c r="B25" s="80"/>
+      <c r="A25" s="77"/>
+      <c r="B25" s="77"/>
       <c r="C25" s="27"/>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
       <c r="F25" s="27"/>
     </row>
     <row r="26" spans="1:6" s="10" customFormat="1">
-      <c r="A26" s="80"/>
-      <c r="B26" s="80"/>
+      <c r="A26" s="77"/>
+      <c r="B26" s="77"/>
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
       <c r="E26" s="27"/>
       <c r="F26" s="27"/>
     </row>
     <row r="27" spans="1:6" s="10" customFormat="1">
-      <c r="A27" s="80"/>
-      <c r="B27" s="80"/>
+      <c r="A27" s="77"/>
+      <c r="B27" s="77"/>
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
       <c r="E27" s="27"/>
       <c r="F27" s="27"/>
     </row>
     <row r="28" spans="1:6" s="10" customFormat="1">
-      <c r="A28" s="80"/>
-      <c r="B28" s="80"/>
+      <c r="A28" s="77"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="27"/>
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
       <c r="F28" s="27"/>
     </row>
     <row r="29" spans="1:6" s="10" customFormat="1">
-      <c r="A29" s="80"/>
-      <c r="B29" s="80"/>
+      <c r="A29" s="77"/>
+      <c r="B29" s="77"/>
       <c r="C29" s="27"/>
       <c r="D29" s="27"/>
       <c r="E29" s="27"/>
       <c r="F29" s="27"/>
     </row>
     <row r="30" spans="1:6" s="10" customFormat="1">
-      <c r="A30" s="80"/>
-      <c r="B30" s="80"/>
+      <c r="A30" s="77"/>
+      <c r="B30" s="77"/>
       <c r="C30" s="27"/>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
       <c r="F30" s="27"/>
     </row>
     <row r="31" spans="1:6" s="10" customFormat="1">
-      <c r="A31" s="80"/>
-      <c r="B31" s="80"/>
+      <c r="A31" s="77"/>
+      <c r="B31" s="77"/>
       <c r="C31" s="27"/>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
       <c r="F31" s="27"/>
     </row>
     <row r="32" spans="1:6" s="10" customFormat="1">
-      <c r="A32" s="80"/>
-      <c r="B32" s="80"/>
+      <c r="A32" s="77"/>
+      <c r="B32" s="77"/>
       <c r="C32" s="27"/>
       <c r="D32" s="27"/>
       <c r="E32" s="27"/>
       <c r="F32" s="27"/>
     </row>
     <row r="33" spans="1:6" s="10" customFormat="1">
-      <c r="A33" s="80"/>
-      <c r="B33" s="80"/>
+      <c r="A33" s="77"/>
+      <c r="B33" s="77"/>
       <c r="C33" s="27"/>
       <c r="D33" s="27"/>
       <c r="E33" s="27"/>
       <c r="F33" s="27"/>
     </row>
     <row r="34" spans="1:6" s="10" customFormat="1">
-      <c r="A34" s="80"/>
-      <c r="B34" s="80"/>
+      <c r="A34" s="77"/>
+      <c r="B34" s="77"/>
       <c r="C34" s="27"/>
       <c r="D34" s="27"/>
       <c r="E34" s="27"/>
       <c r="F34" s="27"/>
     </row>
     <row r="35" spans="1:6" s="10" customFormat="1">
-      <c r="A35" s="80"/>
-      <c r="B35" s="80"/>
+      <c r="A35" s="77"/>
+      <c r="B35" s="77"/>
       <c r="C35" s="27"/>
       <c r="D35" s="27"/>
       <c r="E35" s="27"/>
       <c r="F35" s="27"/>
     </row>
     <row r="36" spans="1:6" s="10" customFormat="1">
-      <c r="A36" s="80"/>
-      <c r="B36" s="80"/>
+      <c r="A36" s="77"/>
+      <c r="B36" s="77"/>
       <c r="C36" s="27"/>
       <c r="D36" s="27"/>
       <c r="E36" s="27"/>
       <c r="F36" s="27"/>
     </row>
     <row r="37" spans="1:6" s="10" customFormat="1">
-      <c r="A37" s="80"/>
-      <c r="B37" s="80"/>
+      <c r="A37" s="77"/>
+      <c r="B37" s="77"/>
       <c r="C37" s="27"/>
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
       <c r="F37" s="27"/>
     </row>
     <row r="38" spans="1:6" s="10" customFormat="1">
-      <c r="A38" s="80"/>
-      <c r="B38" s="80"/>
+      <c r="A38" s="77"/>
+      <c r="B38" s="77"/>
       <c r="C38" s="27"/>
       <c r="D38" s="27"/>
       <c r="E38" s="27"/>
       <c r="F38" s="27"/>
     </row>
     <row r="39" spans="1:6" s="10" customFormat="1">
-      <c r="A39" s="80"/>
-      <c r="B39" s="80"/>
+      <c r="A39" s="77"/>
+      <c r="B39" s="77"/>
       <c r="C39" s="27"/>
       <c r="D39" s="27"/>
       <c r="E39" s="27"/>
       <c r="F39" s="27"/>
     </row>
     <row r="40" spans="1:6" s="10" customFormat="1">
-      <c r="A40" s="80"/>
-      <c r="B40" s="80"/>
+      <c r="A40" s="77"/>
+      <c r="B40" s="77"/>
       <c r="C40" s="27"/>
       <c r="D40" s="27"/>
       <c r="E40" s="27"/>
       <c r="F40" s="27"/>
     </row>
     <row r="41" spans="1:6" s="10" customFormat="1">
-      <c r="A41" s="80"/>
-      <c r="B41" s="80"/>
+      <c r="A41" s="77"/>
+      <c r="B41" s="77"/>
       <c r="C41" s="27"/>
       <c r="D41" s="27"/>
       <c r="E41" s="27"/>
       <c r="F41" s="27"/>
     </row>
     <row r="42" spans="1:6" s="10" customFormat="1">
-      <c r="A42" s="80"/>
-      <c r="B42" s="80"/>
+      <c r="A42" s="77"/>
+      <c r="B42" s="77"/>
       <c r="C42" s="27"/>
       <c r="D42" s="27"/>
       <c r="E42" s="27"/>
       <c r="F42" s="27"/>
     </row>
     <row r="43" spans="1:6" s="10" customFormat="1">
-      <c r="A43" s="80"/>
-      <c r="B43" s="80"/>
+      <c r="A43" s="77"/>
+      <c r="B43" s="77"/>
       <c r="C43" s="27"/>
       <c r="D43" s="27"/>
       <c r="E43" s="27"/>
       <c r="F43" s="27"/>
     </row>
     <row r="44" spans="1:6" s="10" customFormat="1">
-      <c r="A44" s="80"/>
-      <c r="B44" s="80"/>
+      <c r="A44" s="77"/>
+      <c r="B44" s="77"/>
       <c r="C44" s="27"/>
       <c r="D44" s="27"/>
       <c r="E44" s="27"/>
       <c r="F44" s="27"/>
     </row>
     <row r="45" spans="1:6" s="10" customFormat="1">
-      <c r="A45" s="80"/>
-      <c r="B45" s="80"/>
+      <c r="A45" s="77"/>
+      <c r="B45" s="77"/>
       <c r="C45" s="27"/>
       <c r="D45" s="27"/>
       <c r="E45" s="27"/>
       <c r="F45" s="27"/>
     </row>
     <row r="46" spans="1:6" s="10" customFormat="1">
-      <c r="A46" s="80"/>
-      <c r="B46" s="80"/>
+      <c r="A46" s="77"/>
+      <c r="B46" s="77"/>
       <c r="C46" s="27"/>
       <c r="D46" s="27"/>
       <c r="E46" s="27"/>
       <c r="F46" s="27"/>
     </row>
     <row r="47" spans="1:6" s="10" customFormat="1">
-      <c r="A47" s="80"/>
-      <c r="B47" s="80"/>
+      <c r="A47" s="77"/>
+      <c r="B47" s="77"/>
       <c r="C47" s="27"/>
       <c r="D47" s="27"/>
       <c r="E47" s="27"/>
       <c r="F47" s="27"/>
     </row>
     <row r="48" spans="1:6" s="10" customFormat="1">
-      <c r="A48" s="80"/>
-      <c r="B48" s="80"/>
+      <c r="A48" s="77"/>
+      <c r="B48" s="77"/>
       <c r="C48" s="27"/>
       <c r="D48" s="28"/>
       <c r="E48" s="29"/>
       <c r="F48" s="29"/>
     </row>
     <row r="49" spans="1:6" s="10" customFormat="1">
-      <c r="A49" s="80"/>
-      <c r="B49" s="80"/>
+      <c r="A49" s="77"/>
+      <c r="B49" s="77"/>
       <c r="C49" s="27"/>
       <c r="D49" s="28"/>
       <c r="E49" s="29"/>
       <c r="F49" s="29"/>
     </row>
     <row r="50" spans="1:6" s="10" customFormat="1">
-      <c r="A50" s="80"/>
-      <c r="B50" s="80"/>
+      <c r="A50" s="77"/>
+      <c r="B50" s="77"/>
       <c r="C50" s="27"/>
       <c r="D50" s="28"/>
       <c r="E50" s="29"/>
       <c r="F50" s="29"/>
     </row>
     <row r="51" spans="1:6" s="10" customFormat="1">
-      <c r="A51" s="80"/>
-      <c r="B51" s="80"/>
+      <c r="A51" s="77"/>
+      <c r="B51" s="77"/>
       <c r="C51" s="27"/>
       <c r="D51" s="28"/>
       <c r="E51" s="29"/>
       <c r="F51" s="29"/>
     </row>
     <row r="52" spans="1:6" s="10" customFormat="1">
-      <c r="A52" s="80"/>
-      <c r="B52" s="80"/>
+      <c r="A52" s="77"/>
+      <c r="B52" s="77"/>
       <c r="C52" s="27"/>
       <c r="D52" s="28"/>
       <c r="E52" s="29"/>
       <c r="F52" s="29"/>
     </row>
     <row r="53" spans="1:6" s="10" customFormat="1">
-      <c r="A53" s="80"/>
-      <c r="B53" s="80"/>
+      <c r="A53" s="77"/>
+      <c r="B53" s="77"/>
       <c r="C53" s="27"/>
       <c r="D53" s="28"/>
       <c r="E53" s="29"/>
@@ -3318,41 +3313,13 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A6:F6"/>
@@ -3365,15 +3332,43 @@
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3381,10 +3376,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="1a638d2c-e7c0-419c-9191-e92086f67d97">
@@ -3395,7 +3386,20 @@
 </p:properties>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006C2685AC3E5C784C94699E6BCD3719C2" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bc4032ed2b9525712665d7b053f58e3c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a638d2c-e7c0-419c-9191-e92086f67d97" xmlns:ns3="84e25877-5f26-4dc3-9598-48e40fb4ec5c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60642ebedafdd5f29702615754875760" ns2:_="" ns3:_="">
     <xsd:import namespace="1a638d2c-e7c0-419c-9191-e92086f67d97"/>
@@ -3626,24 +3630,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D54ED65-933A-4F90-B95A-15C952E0CAEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1336CC8-439A-433F-AFCD-D3738BD4CF84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3654,7 +3641,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D54ED65-933A-4F90-B95A-15C952E0CAEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{433CEB9C-4DCB-4DF9-8E44-99AD43459D1C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1E225A3-DBF5-416D-8482-D016D280651E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3671,12 +3674,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{433CEB9C-4DCB-4DF9-8E44-99AD43459D1C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>